<commit_message>
updated html css js front end
</commit_message>
<xml_diff>
--- a/nodejs/data/chinese_food_menu_withoutID.xlsx
+++ b/nodejs/data/chinese_food_menu_withoutID.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kennethdouglasslai/teckyC28/c28-bad-proj-07-sw/nodejs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF74B93-465F-134D-95F8-0CD56A841B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C9D4F9-4E0C-FE4A-A859-5D3D9E0FCF7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19740" xr2:uid="{4A62DA01-8191-C04B-B16E-B508969625CC}"/>
   </bookViews>
@@ -242,10 +242,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>銀芽肉絲 炒麵</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>麵</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -371,6 +367,10 @@
   </si>
   <si>
     <t>薯皇</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>銀芽肉絲炒麵</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -806,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D1F953-B570-DF4B-B939-D2296740F01A}">
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -832,13 +832,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
       <c r="D2" s="3">
         <v>60</v>
@@ -846,10 +846,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>2</v>
@@ -860,13 +860,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" s="3">
         <v>60</v>
@@ -874,10 +874,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>3</v>
@@ -888,10 +888,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>4</v>
@@ -902,10 +902,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>5</v>
@@ -916,13 +916,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D8" s="3">
         <v>60</v>
@@ -930,10 +930,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>6</v>
@@ -944,10 +944,10 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>7</v>
@@ -958,10 +958,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>8</v>
@@ -972,10 +972,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>9</v>
@@ -986,10 +986,10 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>10</v>
@@ -1000,10 +1000,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>11</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D15" s="3">
         <v>65</v>
@@ -1028,10 +1028,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>12</v>
@@ -1042,10 +1042,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>13</v>
@@ -1056,10 +1056,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>14</v>
@@ -1070,10 +1070,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>15</v>
@@ -1084,10 +1084,10 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>16</v>
@@ -1098,10 +1098,10 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>17</v>
@@ -1112,10 +1112,10 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>18</v>
@@ -1126,10 +1126,10 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>19</v>
@@ -1140,10 +1140,10 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>20</v>
@@ -1154,10 +1154,10 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>21</v>
@@ -1168,10 +1168,10 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>22</v>
@@ -1182,10 +1182,10 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>23</v>
@@ -1196,13 +1196,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D28" s="3">
         <v>75</v>
@@ -1210,10 +1210,10 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>24</v>
@@ -1224,10 +1224,10 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>25</v>
@@ -1238,10 +1238,10 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>26</v>
@@ -1252,10 +1252,10 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>27</v>
@@ -1266,10 +1266,10 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>28</v>
@@ -1280,10 +1280,10 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>29</v>
@@ -1294,10 +1294,10 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>30</v>
@@ -1308,10 +1308,10 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>31</v>
@@ -1322,10 +1322,10 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>32</v>
@@ -1336,10 +1336,10 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>33</v>
@@ -1350,10 +1350,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>34</v>
@@ -1364,10 +1364,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>35</v>
@@ -1378,10 +1378,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>36</v>
@@ -1392,10 +1392,10 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>37</v>
@@ -1406,10 +1406,10 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>38</v>
@@ -1420,10 +1420,10 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>39</v>
@@ -1434,10 +1434,10 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>40</v>
@@ -1448,13 +1448,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D46" s="3">
         <v>45</v>
@@ -1462,10 +1462,10 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>41</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D48" s="3">
         <v>45</v>
@@ -1490,10 +1490,10 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>42</v>
@@ -1504,10 +1504,10 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>43</v>
@@ -1518,13 +1518,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D51" s="3">
         <v>35</v>
@@ -1532,10 +1532,10 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>44</v>
@@ -1546,10 +1546,10 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>45</v>
@@ -1560,10 +1560,10 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>46</v>
@@ -1574,10 +1574,10 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>47</v>
@@ -1588,10 +1588,10 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>48</v>
@@ -1602,10 +1602,10 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>49</v>
@@ -1616,10 +1616,10 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>50</v>
@@ -1630,10 +1630,10 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>51</v>
@@ -1644,10 +1644,10 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>52</v>

</xml_diff>